<commit_message>
modified:   config.py 	modified:   libs.py 	modified:   main.py 	modified:   source.xlsx
</commit_message>
<xml_diff>
--- a/source.xlsx
+++ b/source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karae\Documents\Git\phase_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BB4FE8-77FF-4883-9F1B-70862CE4061C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C573DFB-CBD5-4285-A769-F3D5539D9374}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2160,7 +2160,7 @@
   <dimension ref="A1:I157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>

</xml_diff>